<commit_message>
Thêm câu 10 khảo sát để dễ tổng hợp.
</commit_message>
<xml_diff>
--- a/PA5/KhaoSat/Tong hop.xlsx
+++ b/PA5/KhaoSat/Tong hop.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4506"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
@@ -11,12 +11,12 @@
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="124519"/>
+  <calcPr calcId="125725"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="59">
   <si>
     <t>Đáp án đánh số tứ nhỏ đến lớn ứng với không hài lòng đến cực kỳ hài lòng</t>
   </si>
@@ -187,6 +187,12 @@
   </si>
   <si>
     <t>Rất dễ dùng, không cần học cũng dùng được</t>
+  </si>
+  <si>
+    <t>Câu 10</t>
+  </si>
+  <si>
+    <t>Góp ý của bạn cho trang web (chỉ cần liệt kê 1 hoặc 2 cái là được)</t>
   </si>
 </sst>
 </file>
@@ -197,7 +203,7 @@
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="Arial"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -205,7 +211,7 @@
       <b/>
       <sz val="11"/>
       <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
+      <name val="Arial"/>
       <family val="2"/>
       <charset val="163"/>
       <scheme val="minor"/>
@@ -214,7 +220,7 @@
       <b/>
       <sz val="11"/>
       <color rgb="FF0070C0"/>
-      <name val="Calibri"/>
+      <name val="Arial"/>
       <family val="2"/>
       <charset val="163"/>
       <scheme val="minor"/>
@@ -223,7 +229,7 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="Arial"/>
       <family val="2"/>
       <charset val="163"/>
       <scheme val="minor"/>
@@ -231,7 +237,7 @@
     <font>
       <sz val="11"/>
       <color rgb="FFC00000"/>
-      <name val="Calibri"/>
+      <name val="Arial"/>
       <family val="2"/>
       <charset val="163"/>
       <scheme val="minor"/>
@@ -239,7 +245,7 @@
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="Arial"/>
       <family val="2"/>
       <charset val="163"/>
       <scheme val="minor"/>
@@ -267,9 +273,6 @@
   </cellStyleXfs>
   <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -277,10 +280,13 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -577,41 +583,41 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:D33"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="B18" sqref="B18"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D28" sqref="D28"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
-    <col min="2" max="2" width="78.28515625" customWidth="1"/>
-    <col min="3" max="3" width="10.7109375" customWidth="1"/>
+    <col min="2" max="2" width="78.25" customWidth="1"/>
+    <col min="3" max="3" width="10.75" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:4" ht="15">
+      <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1"/>
-      <c r="C1" s="1"/>
-      <c r="D1" s="1"/>
-    </row>
-    <row r="2" spans="1:4">
-      <c r="A2" s="2" t="s">
+      <c r="B1" s="5"/>
+      <c r="C1" s="5"/>
+      <c r="D1" s="5"/>
+    </row>
+    <row r="2" spans="1:4" ht="15">
+      <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="3"/>
-      <c r="C2" s="3"/>
-      <c r="D2" s="3"/>
-    </row>
-    <row r="3" spans="1:4">
-      <c r="A3" s="4" t="s">
+      <c r="B2" s="2"/>
+      <c r="C2" s="2"/>
+      <c r="D2" s="2"/>
+    </row>
+    <row r="3" spans="1:4" ht="15">
+      <c r="A3" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="5" t="s">
+      <c r="B3" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="C3" s="5"/>
-      <c r="D3" s="5"/>
+      <c r="C3" s="6"/>
+      <c r="D3" s="6"/>
     </row>
     <row r="4" spans="1:4">
       <c r="A4" t="s">
@@ -656,7 +662,7 @@
       </c>
     </row>
     <row r="7" spans="1:4">
-      <c r="A7" s="6">
+      <c r="A7" s="4">
         <v>3</v>
       </c>
       <c r="B7" t="s">
@@ -955,6 +961,12 @@
       </c>
       <c r="B28" t="s">
         <v>45</v>
+      </c>
+      <c r="C28" t="s">
+        <v>57</v>
+      </c>
+      <c r="D28" t="s">
+        <v>58</v>
       </c>
     </row>
     <row r="29" spans="1:4">
@@ -1012,7 +1024,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1024,7 +1036,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Chỉnh sửa file tổng hợp.
</commit_message>
<xml_diff>
--- a/PA5/KhaoSat/Tong hop.xlsx
+++ b/PA5/KhaoSat/Tong hop.xlsx
@@ -7,22 +7,14 @@
     <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
-    <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
+    <sheet name="DanhGia" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="125725"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="59">
-  <si>
-    <t>Đáp án đánh số tứ nhỏ đến lớn ứng với không hài lòng đến cực kỳ hài lòng</t>
-  </si>
-  <si>
-    <t>Bạn chọn đáp nào thì chỉ cần bôi đen con số là được. Ví dụ câu 1, chọn đáp án 5, chọn ô có số 5, nhấn Ctrl+B là xong</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="74">
   <si>
     <t>*</t>
   </si>
@@ -48,9 +40,6 @@
     <t>Hoàn toàn không thỏa mãn</t>
   </si>
   <si>
-    <t>Một vài thông tin không có.</t>
-  </si>
-  <si>
     <t>Không thỏa mãn</t>
   </si>
   <si>
@@ -81,9 +70,6 @@
     <t>Rất tệ</t>
   </si>
   <si>
-    <t xml:space="preserve">hoàn toàn không </t>
-  </si>
-  <si>
     <t>Tệ</t>
   </si>
   <si>
@@ -105,21 +91,12 @@
     <t>Câu 8</t>
   </si>
   <si>
-    <t>Hoàn toàn không có.</t>
-  </si>
-  <si>
-    <t>không có</t>
-  </si>
-  <si>
     <t>Tương đối</t>
   </si>
   <si>
     <t>Khá tốt</t>
   </si>
   <si>
-    <t>Hoàn toàn.</t>
-  </si>
-  <si>
     <t>Câu 4</t>
   </si>
   <si>
@@ -162,15 +139,9 @@
     <t>Cực kỳ khó thực hiện</t>
   </si>
   <si>
-    <t>khó thực hiện</t>
-  </si>
-  <si>
     <t>Hài lòng</t>
   </si>
   <si>
-    <t>rất hài lòng</t>
-  </si>
-  <si>
     <t>Rất tuyệt</t>
   </si>
   <si>
@@ -193,13 +164,85 @@
   </si>
   <si>
     <t>Góp ý của bạn cho trang web (chỉ cần liệt kê 1 hoặc 2 cái là được)</t>
+  </si>
+  <si>
+    <t>10 câu hỏi, đáp án đánh số tứ nhỏ đến lớn ứng với không hài lòng đến cực kỳ hài lòng</t>
+  </si>
+  <si>
+    <t>MSSV</t>
+  </si>
+  <si>
+    <t>0812000</t>
+  </si>
+  <si>
+    <t>Họ tên</t>
+  </si>
+  <si>
+    <t>Nguyễn Văn A</t>
+  </si>
+  <si>
+    <t>Email</t>
+  </si>
+  <si>
+    <t>abc@gmail.com</t>
+  </si>
+  <si>
+    <t>Bước 1: Điền vài thông tin của bạn, thông tin này để đảm bảo rằng bạn có học trong trường ĐHKHTN và để kiểm tra lại khi cần</t>
+  </si>
+  <si>
+    <t>http://www.mediafire.com/download.php?unpxablg17l0749</t>
+  </si>
+  <si>
+    <t>http://www.mediafire.com/download.php?ljvg1m44bloolq1</t>
+  </si>
+  <si>
+    <t>Bước 2: download 1 trong 2 cái sau về</t>
+  </si>
+  <si>
+    <t>Các file html, mở trên firefox, không có liên kết giữa các màn hình (4.2 MB)</t>
+  </si>
+  <si>
+    <t>Bước 3: bạn chọn đáp nào thì chỉ cần bôi đen con số là được. Ví dụ câu 1, chọn đáp án 5, chọn ô có số 5, nhấn Ctrl+B là xong</t>
+  </si>
+  <si>
+    <t>Hình chụp các màn hình, có ghi chú liên kết giữa các màn hình (2.4 MB)</t>
+  </si>
+  <si>
+    <t>B4: cảm ơn bạn, giờ bạn chỉ cần gửi lại file này là xong</t>
+  </si>
+  <si>
+    <t>Một vài thông tin không có</t>
+  </si>
+  <si>
+    <t>Rất xấu</t>
+  </si>
+  <si>
+    <t>Hơi xấu</t>
+  </si>
+  <si>
+    <t>Rất đẹp</t>
+  </si>
+  <si>
+    <t>Hoàn toàn không</t>
+  </si>
+  <si>
+    <t>không thân thiện lắm</t>
+  </si>
+  <si>
+    <t>Khó thực hiện</t>
+  </si>
+  <si>
+    <t>Rất hài lòng</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Hoàn toàn không </t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="6">
+  <fonts count="8">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -236,7 +279,21 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FFC00000"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="163"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <name val="Arial"/>
       <family val="2"/>
       <charset val="163"/>
@@ -244,7 +301,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FFFF0000"/>
       <name val="Arial"/>
       <family val="2"/>
       <charset val="163"/>
@@ -268,10 +325,14 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="top"/>
+      <protection locked="0"/>
+    </xf>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -280,15 +341,21 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -581,463 +648,507 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D33"/>
+  <dimension ref="A1:D41"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D28" sqref="D28"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
-    <col min="2" max="2" width="78.25" customWidth="1"/>
+    <col min="2" max="2" width="62" customWidth="1"/>
     <col min="3" max="3" width="10.75" customWidth="1"/>
+    <col min="4" max="4" width="65.25" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="15">
-      <c r="A1" s="5" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="5"/>
-      <c r="C1" s="5"/>
-      <c r="D1" s="5"/>
-    </row>
-    <row r="2" spans="1:4" ht="15">
-      <c r="A2" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="B2" s="2"/>
-      <c r="C2" s="2"/>
-      <c r="D2" s="2"/>
-    </row>
-    <row r="3" spans="1:4" ht="15">
-      <c r="A3" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="B3" s="6" t="s">
-        <v>3</v>
-      </c>
-      <c r="C3" s="6"/>
-      <c r="D3" s="6"/>
+      <c r="A1" s="1" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4">
+      <c r="A2" t="s">
+        <v>51</v>
+      </c>
+      <c r="B2" s="6" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4">
+      <c r="A3" t="s">
+        <v>53</v>
+      </c>
+      <c r="B3" t="s">
+        <v>54</v>
+      </c>
     </row>
     <row r="4" spans="1:4">
       <c r="A4" t="s">
+        <v>55</v>
+      </c>
+      <c r="B4" s="7" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" ht="15">
+      <c r="A5" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="B5" s="5"/>
+      <c r="C5" s="5"/>
+      <c r="D5" s="5"/>
+    </row>
+    <row r="6" spans="1:4" ht="15">
+      <c r="A6" s="1"/>
+      <c r="B6" t="s">
+        <v>61</v>
+      </c>
+      <c r="C6" s="7" t="s">
+        <v>58</v>
+      </c>
+      <c r="D6" s="5"/>
+    </row>
+    <row r="7" spans="1:4" ht="15">
+      <c r="A7" s="1"/>
+      <c r="B7" s="8" t="s">
+        <v>63</v>
+      </c>
+      <c r="C7" s="7" t="s">
+        <v>59</v>
+      </c>
+      <c r="D7" s="5"/>
+    </row>
+    <row r="8" spans="1:4" ht="15">
+      <c r="A8" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="B8" s="2"/>
+      <c r="C8" s="2"/>
+      <c r="D8" s="2"/>
+    </row>
+    <row r="9" spans="1:4" ht="15">
+      <c r="A9" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B9" s="9" t="s">
+        <v>50</v>
+      </c>
+      <c r="C9" s="9"/>
+      <c r="D9" s="9"/>
+    </row>
+    <row r="10" spans="1:4" ht="15">
+      <c r="A10" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B10" s="9" t="s">
+        <v>1</v>
+      </c>
+      <c r="C10" s="9"/>
+      <c r="D10" s="9"/>
+    </row>
+    <row r="11" spans="1:4">
+      <c r="A11" t="s">
+        <v>2</v>
+      </c>
+      <c r="B11" t="s">
+        <v>3</v>
+      </c>
+      <c r="C11" t="s">
         <v>4</v>
       </c>
-      <c r="B4" t="s">
+      <c r="D11" t="s">
         <v>5</v>
-      </c>
-      <c r="C4" t="s">
-        <v>6</v>
-      </c>
-      <c r="D4" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4">
-      <c r="A5">
-        <v>1</v>
-      </c>
-      <c r="B5" t="s">
-        <v>8</v>
-      </c>
-      <c r="C5">
-        <v>1</v>
-      </c>
-      <c r="D5" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4">
-      <c r="A6">
-        <v>2</v>
-      </c>
-      <c r="B6" t="s">
-        <v>10</v>
-      </c>
-      <c r="C6">
-        <v>2</v>
-      </c>
-      <c r="D6" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4">
-      <c r="A7" s="4">
-        <v>3</v>
-      </c>
-      <c r="B7" t="s">
-        <v>12</v>
-      </c>
-      <c r="C7">
-        <v>3</v>
-      </c>
-      <c r="D7" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4">
-      <c r="A8">
-        <v>4</v>
-      </c>
-      <c r="B8" t="s">
-        <v>13</v>
-      </c>
-      <c r="C8">
-        <v>4</v>
-      </c>
-      <c r="D8" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4">
-      <c r="A9">
-        <v>5</v>
-      </c>
-      <c r="B9" t="s">
-        <v>15</v>
-      </c>
-      <c r="C9">
-        <v>5</v>
-      </c>
-      <c r="D9" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4">
-      <c r="A10" t="s">
-        <v>17</v>
-      </c>
-      <c r="B10" t="s">
-        <v>52</v>
-      </c>
-      <c r="C10" t="s">
-        <v>18</v>
-      </c>
-      <c r="D10" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4">
-      <c r="A11">
-        <v>1</v>
-      </c>
-      <c r="B11" t="s">
-        <v>53</v>
-      </c>
-      <c r="C11">
-        <v>1</v>
-      </c>
-      <c r="D11" t="s">
-        <v>21</v>
       </c>
     </row>
     <row r="12" spans="1:4">
       <c r="A12">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B12" t="s">
-        <v>54</v>
+        <v>6</v>
       </c>
       <c r="C12">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D12" t="s">
-        <v>23</v>
+        <v>7</v>
       </c>
     </row>
     <row r="13" spans="1:4">
       <c r="A13">
+        <v>2</v>
+      </c>
+      <c r="B13" t="s">
+        <v>65</v>
+      </c>
+      <c r="C13">
+        <v>2</v>
+      </c>
+      <c r="D13" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4">
+      <c r="A14" s="4">
         <v>3</v>
       </c>
-      <c r="B13" t="s">
-        <v>12</v>
-      </c>
-      <c r="C13">
+      <c r="B14" t="s">
+        <v>9</v>
+      </c>
+      <c r="C14">
         <v>3</v>
       </c>
-      <c r="D13" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4">
-      <c r="A14">
-        <v>4</v>
-      </c>
-      <c r="B14" t="s">
-        <v>55</v>
-      </c>
-      <c r="C14">
-        <v>4</v>
-      </c>
       <c r="D14" t="s">
-        <v>24</v>
+        <v>9</v>
       </c>
     </row>
     <row r="15" spans="1:4">
       <c r="A15">
+        <v>4</v>
+      </c>
+      <c r="B15" t="s">
+        <v>10</v>
+      </c>
+      <c r="C15">
+        <v>4</v>
+      </c>
+      <c r="D15" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4">
+      <c r="A16">
         <v>5</v>
       </c>
-      <c r="B15" t="s">
-        <v>56</v>
-      </c>
-      <c r="C15">
+      <c r="B16" t="s">
+        <v>12</v>
+      </c>
+      <c r="C16">
         <v>5</v>
       </c>
-      <c r="D15" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4">
-      <c r="A16" t="s">
-        <v>26</v>
-      </c>
-      <c r="B16" t="s">
-        <v>27</v>
-      </c>
-      <c r="C16" t="s">
-        <v>28</v>
-      </c>
       <c r="D16" t="s">
-        <v>37</v>
+        <v>13</v>
       </c>
     </row>
     <row r="17" spans="1:4">
-      <c r="A17">
-        <v>1</v>
+      <c r="A17" t="s">
+        <v>14</v>
       </c>
       <c r="B17" t="s">
-        <v>29</v>
-      </c>
-      <c r="C17">
-        <v>1</v>
+        <v>43</v>
+      </c>
+      <c r="C17" t="s">
+        <v>15</v>
       </c>
       <c r="D17" t="s">
-        <v>38</v>
+        <v>16</v>
       </c>
     </row>
     <row r="18" spans="1:4">
       <c r="A18">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B18" t="s">
-        <v>30</v>
+        <v>44</v>
       </c>
       <c r="C18">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D18" t="s">
-        <v>39</v>
+        <v>73</v>
       </c>
     </row>
     <row r="19" spans="1:4">
       <c r="A19">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B19" t="s">
-        <v>12</v>
+        <v>45</v>
       </c>
       <c r="C19">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D19" t="s">
-        <v>12</v>
+        <v>19</v>
       </c>
     </row>
     <row r="20" spans="1:4">
       <c r="A20">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B20" t="s">
-        <v>31</v>
+        <v>9</v>
       </c>
       <c r="C20">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D20" t="s">
-        <v>41</v>
+        <v>9</v>
       </c>
     </row>
     <row r="21" spans="1:4">
       <c r="A21">
+        <v>4</v>
+      </c>
+      <c r="B21" t="s">
+        <v>46</v>
+      </c>
+      <c r="C21">
+        <v>4</v>
+      </c>
+      <c r="D21" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4">
+      <c r="A22">
         <v>5</v>
       </c>
-      <c r="B21" t="s">
-        <v>33</v>
-      </c>
-      <c r="C21">
+      <c r="B22" t="s">
+        <v>47</v>
+      </c>
+      <c r="C22">
         <v>5</v>
       </c>
-      <c r="D21" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="22" spans="1:4">
-      <c r="A22" t="s">
-        <v>34</v>
-      </c>
-      <c r="B22" t="s">
-        <v>35</v>
-      </c>
-      <c r="C22" t="s">
-        <v>36</v>
-      </c>
       <c r="D22" t="s">
-        <v>46</v>
+        <v>21</v>
       </c>
     </row>
     <row r="23" spans="1:4">
-      <c r="A23">
-        <v>1</v>
+      <c r="A23" t="s">
+        <v>22</v>
       </c>
       <c r="B23" t="s">
-        <v>29</v>
-      </c>
-      <c r="C23">
-        <v>1</v>
+        <v>23</v>
+      </c>
+      <c r="C23" t="s">
+        <v>24</v>
       </c>
       <c r="D23" t="s">
-        <v>20</v>
+        <v>30</v>
       </c>
     </row>
     <row r="24" spans="1:4">
       <c r="A24">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B24" t="s">
-        <v>30</v>
+        <v>66</v>
       </c>
       <c r="C24">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D24" t="s">
-        <v>22</v>
+        <v>31</v>
       </c>
     </row>
     <row r="25" spans="1:4">
       <c r="A25">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B25" t="s">
-        <v>12</v>
+        <v>67</v>
       </c>
       <c r="C25">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D25" t="s">
-        <v>12</v>
+        <v>32</v>
       </c>
     </row>
     <row r="26" spans="1:4">
       <c r="A26">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B26" t="s">
-        <v>40</v>
+        <v>9</v>
       </c>
       <c r="C26">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D26" t="s">
-        <v>32</v>
+        <v>9</v>
       </c>
     </row>
     <row r="27" spans="1:4">
       <c r="A27">
+        <v>4</v>
+      </c>
+      <c r="B27" t="s">
+        <v>25</v>
+      </c>
+      <c r="C27">
+        <v>4</v>
+      </c>
+      <c r="D27" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4">
+      <c r="A28">
         <v>5</v>
       </c>
-      <c r="B27" t="s">
-        <v>42</v>
-      </c>
-      <c r="C27">
+      <c r="B28" t="s">
+        <v>68</v>
+      </c>
+      <c r="C28">
         <v>5</v>
       </c>
-      <c r="D27" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="28" spans="1:4">
-      <c r="A28" t="s">
-        <v>44</v>
-      </c>
-      <c r="B28" t="s">
-        <v>45</v>
-      </c>
-      <c r="C28" t="s">
-        <v>57</v>
-      </c>
       <c r="D28" t="s">
-        <v>58</v>
+        <v>36</v>
       </c>
     </row>
     <row r="29" spans="1:4">
-      <c r="A29">
-        <v>1</v>
+      <c r="A29" t="s">
+        <v>27</v>
       </c>
       <c r="B29" t="s">
-        <v>47</v>
+        <v>28</v>
+      </c>
+      <c r="C29" t="s">
+        <v>29</v>
+      </c>
+      <c r="D29" t="s">
+        <v>39</v>
       </c>
     </row>
     <row r="30" spans="1:4">
       <c r="A30">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B30" t="s">
-        <v>48</v>
+        <v>69</v>
+      </c>
+      <c r="C30">
+        <v>1</v>
+      </c>
+      <c r="D30" t="s">
+        <v>17</v>
       </c>
     </row>
     <row r="31" spans="1:4">
       <c r="A31">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B31" t="s">
-        <v>12</v>
+        <v>70</v>
+      </c>
+      <c r="C31">
+        <v>2</v>
+      </c>
+      <c r="D31" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="32" spans="1:4">
       <c r="A32">
+        <v>3</v>
+      </c>
+      <c r="B32" t="s">
+        <v>9</v>
+      </c>
+      <c r="C32">
+        <v>3</v>
+      </c>
+      <c r="D32" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4">
+      <c r="A33">
         <v>4</v>
       </c>
-      <c r="B32" t="s">
+      <c r="B33" t="s">
+        <v>33</v>
+      </c>
+      <c r="C33">
+        <v>4</v>
+      </c>
+      <c r="D33" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4">
+      <c r="A34">
+        <v>5</v>
+      </c>
+      <c r="B34" t="s">
+        <v>35</v>
+      </c>
+      <c r="C34">
+        <v>5</v>
+      </c>
+      <c r="D34" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4">
+      <c r="A35" t="s">
+        <v>37</v>
+      </c>
+      <c r="B35" t="s">
+        <v>38</v>
+      </c>
+      <c r="C35" t="s">
+        <v>48</v>
+      </c>
+      <c r="D35" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="33" spans="1:2">
-      <c r="A33">
+    <row r="36" spans="1:4">
+      <c r="A36">
+        <v>1</v>
+      </c>
+      <c r="B36" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4">
+      <c r="A37">
+        <v>2</v>
+      </c>
+      <c r="B37" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4">
+      <c r="A38">
+        <v>3</v>
+      </c>
+      <c r="B38" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4">
+      <c r="A39">
+        <v>4</v>
+      </c>
+      <c r="B39" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4">
+      <c r="A40">
         <v>5</v>
       </c>
-      <c r="B33" t="s">
-        <v>50</v>
-      </c>
+      <c r="B40" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" ht="15">
+      <c r="A41" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="B41" s="2"/>
+      <c r="C41" s="2"/>
+      <c r="D41" s="2"/>
     </row>
   </sheetData>
-  <mergeCells count="2">
-    <mergeCell ref="A1:D1"/>
-    <mergeCell ref="B3:D3"/>
-  </mergeCells>
+  <hyperlinks>
+    <hyperlink ref="B4" r:id="rId1"/>
+    <hyperlink ref="C6" r:id="rId2"/>
+    <hyperlink ref="C7" r:id="rId3"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId4"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Chỉnh sửa file tổng hợp: không cần sinh viên KHTN, nếu là người không học CNTT càng tốt.
</commit_message>
<xml_diff>
--- a/PA5/KhaoSat/Tong hop.xlsx
+++ b/PA5/KhaoSat/Tong hop.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="74">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="72">
   <si>
     <t>*</t>
   </si>
@@ -169,12 +169,6 @@
     <t>10 câu hỏi, đáp án đánh số tứ nhỏ đến lớn ứng với không hài lòng đến cực kỳ hài lòng</t>
   </si>
   <si>
-    <t>MSSV</t>
-  </si>
-  <si>
-    <t>0812000</t>
-  </si>
-  <si>
     <t>Họ tên</t>
   </si>
   <si>
@@ -187,9 +181,6 @@
     <t>abc@gmail.com</t>
   </si>
   <si>
-    <t>Bước 1: Điền vài thông tin của bạn, thông tin này để đảm bảo rằng bạn có học trong trường ĐHKHTN và để kiểm tra lại khi cần</t>
-  </si>
-  <si>
     <t>http://www.mediafire.com/download.php?unpxablg17l0749</t>
   </si>
   <si>
@@ -236,6 +227,9 @@
   </si>
   <si>
     <t xml:space="preserve">Hoàn toàn không </t>
+  </si>
+  <si>
+    <t>Bước 1: Điền vài thông tin của bạn, thông tin này để kiểm tra lại khi cần</t>
   </si>
 </sst>
 </file>
@@ -332,7 +326,7 @@
       <protection locked="0"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -345,7 +339,6 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left"/>
     </xf>
@@ -648,7 +641,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D41"/>
+  <dimension ref="A1:D40"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -661,14 +654,14 @@
   <sheetData>
     <row r="1" spans="1:4" ht="15">
       <c r="A1" s="1" t="s">
-        <v>57</v>
+        <v>71</v>
       </c>
     </row>
     <row r="2" spans="1:4">
       <c r="A2" t="s">
         <v>51</v>
       </c>
-      <c r="B2" s="6" t="s">
+      <c r="B2" t="s">
         <v>52</v>
       </c>
     </row>
@@ -676,477 +669,469 @@
       <c r="A3" t="s">
         <v>53</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B3" s="6" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="4" spans="1:4">
-      <c r="A4" t="s">
+    <row r="4" spans="1:4" ht="15">
+      <c r="A4" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="B4" s="5"/>
+      <c r="C4" s="5"/>
+      <c r="D4" s="5"/>
+    </row>
+    <row r="5" spans="1:4" ht="15">
+      <c r="A5" s="1"/>
+      <c r="B5" t="s">
+        <v>58</v>
+      </c>
+      <c r="C5" s="6" t="s">
         <v>55</v>
       </c>
-      <c r="B4" s="7" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" ht="15">
-      <c r="A5" s="1" t="s">
-        <v>60</v>
-      </c>
-      <c r="B5" s="5"/>
-      <c r="C5" s="5"/>
       <c r="D5" s="5"/>
     </row>
     <row r="6" spans="1:4" ht="15">
       <c r="A6" s="1"/>
-      <c r="B6" t="s">
-        <v>61</v>
-      </c>
-      <c r="C6" s="7" t="s">
-        <v>58</v>
+      <c r="B6" s="7" t="s">
+        <v>60</v>
+      </c>
+      <c r="C6" s="6" t="s">
+        <v>56</v>
       </c>
       <c r="D6" s="5"/>
     </row>
     <row r="7" spans="1:4" ht="15">
-      <c r="A7" s="1"/>
-      <c r="B7" s="8" t="s">
-        <v>63</v>
-      </c>
-      <c r="C7" s="7" t="s">
+      <c r="A7" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="D7" s="5"/>
+      <c r="B7" s="2"/>
+      <c r="C7" s="2"/>
+      <c r="D7" s="2"/>
     </row>
     <row r="8" spans="1:4" ht="15">
       <c r="A8" s="1" t="s">
-        <v>62</v>
-      </c>
-      <c r="B8" s="2"/>
-      <c r="C8" s="2"/>
-      <c r="D8" s="2"/>
+        <v>0</v>
+      </c>
+      <c r="B8" s="8" t="s">
+        <v>50</v>
+      </c>
+      <c r="C8" s="8"/>
+      <c r="D8" s="8"/>
     </row>
     <row r="9" spans="1:4" ht="15">
-      <c r="A9" s="1" t="s">
+      <c r="A9" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B9" s="9" t="s">
-        <v>50</v>
-      </c>
-      <c r="C9" s="9"/>
-      <c r="D9" s="9"/>
-    </row>
-    <row r="10" spans="1:4" ht="15">
-      <c r="A10" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="B10" s="9" t="s">
+      <c r="B9" s="8" t="s">
         <v>1</v>
       </c>
-      <c r="C10" s="9"/>
-      <c r="D10" s="9"/>
+      <c r="C9" s="8"/>
+      <c r="D9" s="8"/>
+    </row>
+    <row r="10" spans="1:4">
+      <c r="A10" t="s">
+        <v>2</v>
+      </c>
+      <c r="B10" t="s">
+        <v>3</v>
+      </c>
+      <c r="C10" t="s">
+        <v>4</v>
+      </c>
+      <c r="D10" t="s">
+        <v>5</v>
+      </c>
     </row>
     <row r="11" spans="1:4">
-      <c r="A11" t="s">
-        <v>2</v>
+      <c r="A11">
+        <v>1</v>
       </c>
       <c r="B11" t="s">
-        <v>3</v>
-      </c>
-      <c r="C11" t="s">
-        <v>4</v>
+        <v>6</v>
+      </c>
+      <c r="C11">
+        <v>1</v>
       </c>
       <c r="D11" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
     </row>
     <row r="12" spans="1:4">
       <c r="A12">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B12" t="s">
-        <v>6</v>
+        <v>62</v>
       </c>
       <c r="C12">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D12" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="13" spans="1:4">
-      <c r="A13">
-        <v>2</v>
+      <c r="A13" s="4">
+        <v>3</v>
       </c>
       <c r="B13" t="s">
-        <v>65</v>
+        <v>9</v>
       </c>
       <c r="C13">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D13" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="14" spans="1:4">
-      <c r="A14" s="4">
-        <v>3</v>
+      <c r="A14">
+        <v>4</v>
       </c>
       <c r="B14" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C14">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="D14" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
     </row>
     <row r="15" spans="1:4">
       <c r="A15">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B15" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="C15">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="D15" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
     </row>
     <row r="16" spans="1:4">
-      <c r="A16">
-        <v>5</v>
+      <c r="A16" t="s">
+        <v>14</v>
       </c>
       <c r="B16" t="s">
-        <v>12</v>
-      </c>
-      <c r="C16">
-        <v>5</v>
+        <v>43</v>
+      </c>
+      <c r="C16" t="s">
+        <v>15</v>
       </c>
       <c r="D16" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
     </row>
     <row r="17" spans="1:4">
-      <c r="A17" t="s">
-        <v>14</v>
+      <c r="A17">
+        <v>1</v>
       </c>
       <c r="B17" t="s">
-        <v>43</v>
-      </c>
-      <c r="C17" t="s">
-        <v>15</v>
+        <v>44</v>
+      </c>
+      <c r="C17">
+        <v>1</v>
       </c>
       <c r="D17" t="s">
-        <v>16</v>
+        <v>70</v>
       </c>
     </row>
     <row r="18" spans="1:4">
       <c r="A18">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B18" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="C18">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D18" t="s">
-        <v>73</v>
+        <v>19</v>
       </c>
     </row>
     <row r="19" spans="1:4">
       <c r="A19">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="B19" t="s">
-        <v>45</v>
+        <v>9</v>
       </c>
       <c r="C19">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D19" t="s">
-        <v>19</v>
+        <v>9</v>
       </c>
     </row>
     <row r="20" spans="1:4">
       <c r="A20">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B20" t="s">
-        <v>9</v>
+        <v>46</v>
       </c>
       <c r="C20">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="D20" t="s">
-        <v>9</v>
+        <v>20</v>
       </c>
     </row>
     <row r="21" spans="1:4">
       <c r="A21">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B21" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="C21">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="D21" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
     </row>
     <row r="22" spans="1:4">
-      <c r="A22">
-        <v>5</v>
+      <c r="A22" t="s">
+        <v>22</v>
       </c>
       <c r="B22" t="s">
-        <v>47</v>
-      </c>
-      <c r="C22">
-        <v>5</v>
+        <v>23</v>
+      </c>
+      <c r="C22" t="s">
+        <v>24</v>
       </c>
       <c r="D22" t="s">
-        <v>21</v>
+        <v>30</v>
       </c>
     </row>
     <row r="23" spans="1:4">
-      <c r="A23" t="s">
-        <v>22</v>
+      <c r="A23">
+        <v>1</v>
       </c>
       <c r="B23" t="s">
-        <v>23</v>
-      </c>
-      <c r="C23" t="s">
-        <v>24</v>
+        <v>63</v>
+      </c>
+      <c r="C23">
+        <v>1</v>
       </c>
       <c r="D23" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
     </row>
     <row r="24" spans="1:4">
       <c r="A24">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B24" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="C24">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D24" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
     </row>
     <row r="25" spans="1:4">
       <c r="A25">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="B25" t="s">
-        <v>67</v>
+        <v>9</v>
       </c>
       <c r="C25">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D25" t="s">
-        <v>32</v>
+        <v>9</v>
       </c>
     </row>
     <row r="26" spans="1:4">
       <c r="A26">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B26" t="s">
-        <v>9</v>
+        <v>25</v>
       </c>
       <c r="C26">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="D26" t="s">
-        <v>9</v>
+        <v>34</v>
       </c>
     </row>
     <row r="27" spans="1:4">
       <c r="A27">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B27" t="s">
-        <v>25</v>
+        <v>65</v>
       </c>
       <c r="C27">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="D27" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
     </row>
     <row r="28" spans="1:4">
-      <c r="A28">
-        <v>5</v>
+      <c r="A28" t="s">
+        <v>27</v>
       </c>
       <c r="B28" t="s">
-        <v>68</v>
-      </c>
-      <c r="C28">
-        <v>5</v>
+        <v>28</v>
+      </c>
+      <c r="C28" t="s">
+        <v>29</v>
       </c>
       <c r="D28" t="s">
-        <v>36</v>
+        <v>39</v>
       </c>
     </row>
     <row r="29" spans="1:4">
-      <c r="A29" t="s">
-        <v>27</v>
+      <c r="A29">
+        <v>1</v>
       </c>
       <c r="B29" t="s">
-        <v>28</v>
-      </c>
-      <c r="C29" t="s">
-        <v>29</v>
+        <v>66</v>
+      </c>
+      <c r="C29">
+        <v>1</v>
       </c>
       <c r="D29" t="s">
-        <v>39</v>
+        <v>17</v>
       </c>
     </row>
     <row r="30" spans="1:4">
       <c r="A30">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B30" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="C30">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D30" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
     </row>
     <row r="31" spans="1:4">
       <c r="A31">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="B31" t="s">
-        <v>70</v>
+        <v>9</v>
       </c>
       <c r="C31">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D31" t="s">
-        <v>18</v>
+        <v>9</v>
       </c>
     </row>
     <row r="32" spans="1:4">
       <c r="A32">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B32" t="s">
-        <v>9</v>
+        <v>33</v>
       </c>
       <c r="C32">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="D32" t="s">
-        <v>9</v>
+        <v>26</v>
       </c>
     </row>
     <row r="33" spans="1:4">
       <c r="A33">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B33" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="C33">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="D33" t="s">
-        <v>26</v>
+        <v>42</v>
       </c>
     </row>
     <row r="34" spans="1:4">
-      <c r="A34">
-        <v>5</v>
+      <c r="A34" t="s">
+        <v>37</v>
       </c>
       <c r="B34" t="s">
-        <v>35</v>
-      </c>
-      <c r="C34">
-        <v>5</v>
+        <v>38</v>
+      </c>
+      <c r="C34" t="s">
+        <v>48</v>
       </c>
       <c r="D34" t="s">
-        <v>42</v>
+        <v>49</v>
       </c>
     </row>
     <row r="35" spans="1:4">
-      <c r="A35" t="s">
-        <v>37</v>
+      <c r="A35">
+        <v>1</v>
       </c>
       <c r="B35" t="s">
-        <v>38</v>
-      </c>
-      <c r="C35" t="s">
-        <v>48</v>
-      </c>
-      <c r="D35" t="s">
-        <v>49</v>
+        <v>40</v>
       </c>
     </row>
     <row r="36" spans="1:4">
       <c r="A36">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B36" t="s">
-        <v>40</v>
+        <v>68</v>
       </c>
     </row>
     <row r="37" spans="1:4">
       <c r="A37">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="B37" t="s">
-        <v>71</v>
+        <v>9</v>
       </c>
     </row>
     <row r="38" spans="1:4">
       <c r="A38">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B38" t="s">
-        <v>9</v>
+        <v>41</v>
       </c>
     </row>
     <row r="39" spans="1:4">
       <c r="A39">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B39" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="40" spans="1:4">
-      <c r="A40">
-        <v>5</v>
-      </c>
-      <c r="B40" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="41" spans="1:4" ht="15">
-      <c r="A41" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="B41" s="2"/>
-      <c r="C41" s="2"/>
-      <c r="D41" s="2"/>
+        <v>69</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" ht="15">
+      <c r="A40" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="B40" s="2"/>
+      <c r="C40" s="2"/>
+      <c r="D40" s="2"/>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B4" r:id="rId1"/>
-    <hyperlink ref="C6" r:id="rId2"/>
-    <hyperlink ref="C7" r:id="rId3"/>
+    <hyperlink ref="B3" r:id="rId1"/>
+    <hyperlink ref="C5" r:id="rId2"/>
+    <hyperlink ref="C6" r:id="rId3"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId4"/>

</xml_diff>